<commit_message>
added thumbnail and made major headway on excel post
</commit_message>
<xml_diff>
--- a/posts/excel-wings/test.xlsx
+++ b/posts/excel-wings/test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pamerkha\Documents\Projects\peter-amerkhanian.github.io\posts\excel-wings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BC09C3-AB8C-4870-B411-49E392D92F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCCA09F-63BE-4CA7-B701-C5CCB04BE6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="6300" windowWidth="18870" windowHeight="9180" xr2:uid="{E852D0C5-15DA-4DD9-8BD7-DADA833F5F8F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A24C5838-BE08-47D1-879B-43148CC9E59E}"/>
   </bookViews>
   <sheets>
-    <sheet name="function_sheet" sheetId="2" r:id="rId1"/>
+    <sheet name="function_sheet" sheetId="3" r:id="rId1"/>
+    <sheet name="first_test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>Payment Method</t>
   </si>
@@ -135,8 +136,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -471,7 +472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0517271E-E6EC-4711-8953-D4A0C218D5F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56E8D73-717F-4FA1-8B99-83292B3394DF}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -502,7 +503,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -510,16 +511,16 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>15016</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>17026.47</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>18208.16</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>18242.88</v>
       </c>
       <c r="F2" s="5">
@@ -530,16 +531,16 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>16074.92</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>10960.64</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>16052.85</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>20187.25</v>
       </c>
       <c r="F3" s="5">
@@ -550,16 +551,16 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>14032.23</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>17325.96</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>14363.99</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>17188.669999999998</v>
       </c>
       <c r="F4" s="5">
@@ -570,16 +571,16 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>14143.84</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>15108.84</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>16852.170000000002</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>12065.14</v>
       </c>
       <c r="F5" s="5">
@@ -587,7 +588,148 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>59266.989999999991</v>
+      </c>
+      <c r="C6" s="5">
+        <v>60421.91</v>
+      </c>
+      <c r="D6" s="5">
+        <v>65477.17</v>
+      </c>
+      <c r="E6" s="5">
+        <v>67683.94</v>
+      </c>
+      <c r="F6" s="5">
+        <v>252850.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7077BB01-83B7-4079-81B7-5D2823E2F4C4}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4">
+        <v>15016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>17026.47</v>
+      </c>
+      <c r="D2" s="4">
+        <v>18208.16</v>
+      </c>
+      <c r="E2" s="4">
+        <v>18242.88</v>
+      </c>
+      <c r="F2" s="5">
+        <v>68493.510000000009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4">
+        <v>16074.92</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10960.64</v>
+      </c>
+      <c r="D3" s="4">
+        <v>16052.85</v>
+      </c>
+      <c r="E3" s="4">
+        <v>20187.25</v>
+      </c>
+      <c r="F3" s="5">
+        <v>63275.659999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4">
+        <v>14032.23</v>
+      </c>
+      <c r="C4" s="4">
+        <v>17325.96</v>
+      </c>
+      <c r="D4" s="4">
+        <v>14363.99</v>
+      </c>
+      <c r="E4" s="4">
+        <v>17188.669999999998</v>
+      </c>
+      <c r="F4" s="5">
+        <v>62910.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4">
+        <v>14143.84</v>
+      </c>
+      <c r="C5" s="4">
+        <v>15108.84</v>
+      </c>
+      <c r="D5" s="4">
+        <v>16852.170000000002</v>
+      </c>
+      <c r="E5" s="4">
+        <v>12065.14</v>
+      </c>
+      <c r="F5" s="5">
+        <v>58169.990000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5">

</xml_diff>

<commit_message>
more updates to excel post
</commit_message>
<xml_diff>
--- a/posts/excel-wings/test.xlsx
+++ b/posts/excel-wings/test.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pamerkha\Documents\Projects\peter-amerkhanian.github.io\posts\excel-wings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EF0F70-B22F-46E4-B357-60BF2630D734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6D3124-8333-4F82-80A9-3865389512D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A24C5838-BE08-47D1-879B-43148CC9E59E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4ADFEFA9-5091-4162-85D5-BCCE86E186F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="function_sheet" sheetId="3" r:id="rId1"/>
-    <sheet name="first_test" sheetId="2" r:id="rId2"/>
+    <sheet name="complex_sheet" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,24 +36,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+  <si>
+    <t>Discretionary</t>
+  </si>
+  <si>
+    <t>Necessity</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
   <si>
     <t>Payment Method</t>
   </si>
   <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
     <t>Clothing</t>
   </si>
   <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>Entertainment</t>
-  </si>
-  <si>
     <t>Groceries</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>Cash</t>
@@ -73,39 +78,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -113,32 +102,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,284 +442,281 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56E8D73-717F-4FA1-8B99-83292B3394DF}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C06E0F-56AA-455B-AB23-4653C106B410}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
-        <v>15016</v>
-      </c>
-      <c r="C2" s="4">
-        <v>17026.47</v>
-      </c>
-      <c r="D2" s="4">
-        <v>18208.16</v>
-      </c>
-      <c r="E2" s="4">
-        <v>18242.88</v>
-      </c>
-      <c r="F2" s="5">
-        <v>68493.510000000009</v>
+      <c r="F2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4">
-        <v>16074.92</v>
-      </c>
-      <c r="C3" s="4">
-        <v>10960.64</v>
-      </c>
-      <c r="D3" s="4">
-        <v>16052.85</v>
-      </c>
-      <c r="E3" s="4">
-        <v>20187.25</v>
-      </c>
-      <c r="F3" s="5">
-        <v>63275.659999999996</v>
+      <c r="A3" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>5182.41</v>
+      </c>
+      <c r="D3">
+        <v>8661.2800000000007</v>
+      </c>
+      <c r="E3">
+        <v>5709.71</v>
+      </c>
+      <c r="F3">
+        <v>6552.53</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>2976.99</v>
+      </c>
+      <c r="D4">
+        <v>5334.29</v>
+      </c>
+      <c r="E4">
+        <v>5846.53</v>
+      </c>
+      <c r="F4">
+        <v>7983.28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>6997.97</v>
+      </c>
+      <c r="D5">
+        <v>4998.41</v>
+      </c>
+      <c r="E5">
+        <v>4887.8900000000003</v>
+      </c>
+      <c r="F5">
+        <v>5603.41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>5649.27</v>
+      </c>
+      <c r="D6">
+        <v>7034.34</v>
+      </c>
+      <c r="E6">
+        <v>5225.22</v>
+      </c>
+      <c r="F6">
+        <v>3945.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>2025</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4">
-        <v>14032.23</v>
-      </c>
-      <c r="C4" s="4">
-        <v>17325.96</v>
-      </c>
-      <c r="D4" s="4">
-        <v>14363.99</v>
-      </c>
-      <c r="E4" s="4">
-        <v>17188.669999999998</v>
-      </c>
-      <c r="F4" s="5">
-        <v>62910.85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="C7">
+        <v>6148.02</v>
+      </c>
+      <c r="D7">
+        <v>5110.8</v>
+      </c>
+      <c r="E7">
+        <v>4651.67</v>
+      </c>
+      <c r="F7">
+        <v>7717.81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4">
-        <v>14143.84</v>
-      </c>
-      <c r="C5" s="4">
-        <v>15108.84</v>
-      </c>
-      <c r="D5" s="4">
-        <v>16852.170000000002</v>
-      </c>
-      <c r="E5" s="4">
-        <v>12065.14</v>
-      </c>
-      <c r="F5" s="5">
-        <v>58169.990000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5">
-        <v>59266.989999999991</v>
-      </c>
-      <c r="C6" s="5">
-        <v>60421.91</v>
-      </c>
-      <c r="D6" s="5">
-        <v>65477.17</v>
-      </c>
-      <c r="E6" s="5">
-        <v>67683.94</v>
-      </c>
-      <c r="F6" s="5">
-        <v>252850.01</v>
+      <c r="C8">
+        <v>4618.4399999999996</v>
+      </c>
+      <c r="D8">
+        <v>5946.3099999999995</v>
+      </c>
+      <c r="E8">
+        <v>6843.13</v>
+      </c>
+      <c r="F8">
+        <v>5828.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>6606.99</v>
+      </c>
+      <c r="D9">
+        <v>7087.51</v>
+      </c>
+      <c r="E9">
+        <v>5801.2</v>
+      </c>
+      <c r="F9">
+        <v>4554.53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>5220.53</v>
+      </c>
+      <c r="D10">
+        <v>5592.94</v>
+      </c>
+      <c r="E10">
+        <v>6203.22</v>
+      </c>
+      <c r="F10">
+        <v>3442.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>2026</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>5696.04</v>
+      </c>
+      <c r="D11">
+        <v>4436.08</v>
+      </c>
+      <c r="E11">
+        <v>4654.62</v>
+      </c>
+      <c r="F11">
+        <v>3972.54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>3365.21</v>
+      </c>
+      <c r="D12">
+        <v>4772.25</v>
+      </c>
+      <c r="E12">
+        <v>3385.2599999999998</v>
+      </c>
+      <c r="F12">
+        <v>6375.17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>3721</v>
+      </c>
+      <c r="D13">
+        <v>2278.0699999999997</v>
+      </c>
+      <c r="E13">
+        <v>3343.14</v>
+      </c>
+      <c r="F13">
+        <v>7030.73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>4239.04</v>
+      </c>
+      <c r="D14">
+        <v>4224.8900000000003</v>
+      </c>
+      <c r="E14">
+        <v>2715.4</v>
+      </c>
+      <c r="F14">
+        <v>4676.99</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7077BB01-83B7-4079-81B7-5D2823E2F4C4}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4">
-        <v>15016</v>
-      </c>
-      <c r="C2" s="4">
-        <v>17026.47</v>
-      </c>
-      <c r="D2" s="4">
-        <v>18208.16</v>
-      </c>
-      <c r="E2" s="4">
-        <v>18242.88</v>
-      </c>
-      <c r="F2" s="5">
-        <v>68493.510000000009</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4">
-        <v>16074.92</v>
-      </c>
-      <c r="C3" s="4">
-        <v>10960.64</v>
-      </c>
-      <c r="D3" s="4">
-        <v>16052.85</v>
-      </c>
-      <c r="E3" s="4">
-        <v>20187.25</v>
-      </c>
-      <c r="F3" s="5">
-        <v>63275.659999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4">
-        <v>14032.23</v>
-      </c>
-      <c r="C4" s="4">
-        <v>17325.96</v>
-      </c>
-      <c r="D4" s="4">
-        <v>14363.99</v>
-      </c>
-      <c r="E4" s="4">
-        <v>17188.669999999998</v>
-      </c>
-      <c r="F4" s="5">
-        <v>62910.85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4">
-        <v>14143.84</v>
-      </c>
-      <c r="C5" s="4">
-        <v>15108.84</v>
-      </c>
-      <c r="D5" s="4">
-        <v>16852.170000000002</v>
-      </c>
-      <c r="E5" s="4">
-        <v>12065.14</v>
-      </c>
-      <c r="F5" s="5">
-        <v>58169.990000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5">
-        <v>59266.989999999991</v>
-      </c>
-      <c r="C6" s="5">
-        <v>60421.91</v>
-      </c>
-      <c r="D6" s="5">
-        <v>65477.17</v>
-      </c>
-      <c r="E6" s="5">
-        <v>67683.94</v>
-      </c>
-      <c r="F6" s="5">
-        <v>252850.01</v>
-      </c>
-    </row>
-  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated text in excel post
</commit_message>
<xml_diff>
--- a/posts/excel-wings/test.xlsx
+++ b/posts/excel-wings/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pamerkha\Documents\Projects\peter-amerkhanian.github.io\posts\excel-wings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C011C8C-03BB-446E-B232-628C75B06B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C12EE2A-4C99-445A-86B1-D10FBB450A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1D1A1879-38EA-43F8-8786-DE83EAD29D09}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" xr2:uid="{1D1A1879-38EA-43F8-8786-DE83EAD29D09}"/>
   </bookViews>
   <sheets>
     <sheet name="complex_sheet" sheetId="4" r:id="rId1"/>
@@ -158,11 +158,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -508,16 +508,16 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
       <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
@@ -526,36 +526,36 @@
         <v>11</v>
       </c>
       <c r="F1" s="9"/>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>2024</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4">
@@ -576,7 +576,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4">
@@ -597,7 +597,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="4">
@@ -618,7 +618,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="4">
@@ -639,7 +639,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="10">
@@ -662,7 +662,7 @@
       <c r="A8" s="9">
         <v>2025</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4">
@@ -683,7 +683,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="4">
@@ -704,7 +704,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="4">
@@ -725,7 +725,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="4">
@@ -746,7 +746,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="10">
@@ -769,7 +769,7 @@
       <c r="A13" s="9">
         <v>2026</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="4">
@@ -790,7 +790,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="4">
@@ -811,7 +811,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="4">
@@ -832,7 +832,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="4">
@@ -853,7 +853,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="10">
@@ -873,10 +873,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="10">
         <v>60421.91</v>
       </c>
@@ -913,10 +913,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -937,7 +936,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -957,7 +956,7 @@
       <c r="E2" s="4">
         <v>18242.88</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="8">
         <v>68493.509999999995</v>
       </c>
     </row>
@@ -977,7 +976,7 @@
       <c r="E3" s="4">
         <v>20187.25</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="8">
         <v>63275.659999999996</v>
       </c>
     </row>
@@ -997,7 +996,7 @@
       <c r="E4" s="4">
         <v>17188.669999999998</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="8">
         <v>62910.85</v>
       </c>
     </row>
@@ -1017,27 +1016,27 @@
       <c r="E5" s="4">
         <v>12065.14</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="8">
         <v>58169.99</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="8">
         <v>59266.99</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="8">
         <v>60421.91</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="8">
         <v>65477.17</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="8">
         <v>67683.94</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="8">
         <v>252850.01</v>
       </c>
     </row>
@@ -1054,10 +1053,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>